<commit_message>
Ngrams Model Cheeck 3
</commit_message>
<xml_diff>
--- a/data/main-data/Restaurant.xlsx
+++ b/data/main-data/Restaurant.xlsx
@@ -5643,8 +5643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q2060"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C221" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="H218" sqref="H218"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>